<commit_message>
New data for KMC, new format for optimising budgets
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Arusha_v2.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Arusha_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92964936-7048-E649-B211-9ED596F55BB5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0C10D-EAC3-0643-89E0-875757463022}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="50" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <definedName name="PWPop">'[1]Baseline year demographics'!$C$44:$C$47</definedName>
     <definedName name="WRAPop">'[1]Baseline year demographics'!$C$32:$C$35</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -6434,13 +6434,13 @@
     <xf numFmtId="0" fontId="31" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="34" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="739" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="739" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="740">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -8808,38 +8808,38 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="153" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" style="153" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="153"/>
+    <col min="1" max="1" width="17.5" style="152" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="152" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="152"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="154" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="154" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="154" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="156">
+      <c r="B2" s="155">
         <v>329810.39545454545</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="154" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="154"/>
+      <c r="B3" s="153"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13957,7 +13957,7 @@
       <c r="A2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="156" t="s">
         <v>72</v>
       </c>
       <c r="C2" t="s">
@@ -13980,7 +13980,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="152"/>
+      <c r="B3" s="156"/>
       <c r="C3" t="s">
         <v>150</v>
       </c>
@@ -14002,7 +14002,7 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="152"/>
+      <c r="B4" s="156"/>
       <c r="C4" t="s">
         <v>160</v>
       </c>
@@ -14024,7 +14024,7 @@
       <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="156" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -14047,7 +14047,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="152"/>
+      <c r="B6" s="156"/>
       <c r="C6" t="s">
         <v>150</v>
       </c>
@@ -14068,7 +14068,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="152"/>
+      <c r="B7" s="156"/>
       <c r="C7" t="s">
         <v>160</v>
       </c>
@@ -14089,7 +14089,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="156" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -14112,7 +14112,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="152"/>
+      <c r="B9" s="156"/>
       <c r="C9" t="s">
         <v>150</v>
       </c>
@@ -14133,7 +14133,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="152"/>
+      <c r="B10" s="156"/>
       <c r="C10" t="s">
         <v>160</v>
       </c>
@@ -14154,7 +14154,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="156" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
@@ -14177,7 +14177,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="152"/>
+      <c r="B12" s="156"/>
       <c r="C12" t="s">
         <v>150</v>
       </c>
@@ -14198,7 +14198,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="152"/>
+      <c r="B13" s="156"/>
       <c r="C13" t="s">
         <v>160</v>
       </c>
@@ -14219,7 +14219,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B14" s="152" t="s">
+      <c r="B14" s="156" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
@@ -14242,7 +14242,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="152"/>
+      <c r="B15" s="156"/>
       <c r="C15" t="s">
         <v>150</v>
       </c>
@@ -14263,7 +14263,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="152"/>
+      <c r="B16" s="156"/>
       <c r="C16" t="s">
         <v>160</v>
       </c>
@@ -14317,7 +14317,7 @@
       <c r="A19" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="152" t="s">
+      <c r="B19" s="156" t="s">
         <v>72</v>
       </c>
       <c r="C19" t="s">
@@ -14340,7 +14340,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="152"/>
+      <c r="B20" s="156"/>
       <c r="C20" t="s">
         <v>150</v>
       </c>
@@ -14361,7 +14361,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="152"/>
+      <c r="B21" s="156"/>
       <c r="C21" t="s">
         <v>160</v>
       </c>
@@ -14382,7 +14382,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="152" t="s">
+      <c r="B22" s="156" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
@@ -14405,7 +14405,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="152"/>
+      <c r="B23" s="156"/>
       <c r="C23" t="s">
         <v>150</v>
       </c>
@@ -14426,7 +14426,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="152"/>
+      <c r="B24" s="156"/>
       <c r="C24" t="s">
         <v>160</v>
       </c>
@@ -14447,7 +14447,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="152" t="s">
+      <c r="B25" s="156" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
@@ -14470,7 +14470,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="152"/>
+      <c r="B26" s="156"/>
       <c r="C26" t="s">
         <v>150</v>
       </c>
@@ -14491,7 +14491,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="152"/>
+      <c r="B27" s="156"/>
       <c r="C27" t="s">
         <v>160</v>
       </c>
@@ -14512,7 +14512,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B28" s="152" t="s">
+      <c r="B28" s="156" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
@@ -14535,7 +14535,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B29" s="152"/>
+      <c r="B29" s="156"/>
       <c r="C29" t="s">
         <v>150</v>
       </c>
@@ -14556,7 +14556,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B30" s="152"/>
+      <c r="B30" s="156"/>
       <c r="C30" t="s">
         <v>160</v>
       </c>
@@ -14577,7 +14577,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B31" s="152" t="s">
+      <c r="B31" s="156" t="s">
         <v>9</v>
       </c>
       <c r="C31" t="s">
@@ -14600,7 +14600,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B32" s="152"/>
+      <c r="B32" s="156"/>
       <c r="C32" t="s">
         <v>150</v>
       </c>
@@ -14621,7 +14621,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B33" s="152"/>
+      <c r="B33" s="156"/>
       <c r="C33" t="s">
         <v>160</v>
       </c>
@@ -14668,7 +14668,7 @@
       <c r="A36" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="152" t="s">
+      <c r="B36" s="156" t="s">
         <v>72</v>
       </c>
       <c r="C36" t="s">
@@ -14691,7 +14691,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B37" s="152"/>
+      <c r="B37" s="156"/>
       <c r="C37" t="s">
         <v>150</v>
       </c>
@@ -14712,7 +14712,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B38" s="152"/>
+      <c r="B38" s="156"/>
       <c r="C38" t="s">
         <v>160</v>
       </c>
@@ -14734,7 +14734,7 @@
       <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="156" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
@@ -14757,7 +14757,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B40" s="152"/>
+      <c r="B40" s="156"/>
       <c r="C40" t="s">
         <v>150</v>
       </c>
@@ -14778,7 +14778,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B41" s="152"/>
+      <c r="B41" s="156"/>
       <c r="C41" t="s">
         <v>160</v>
       </c>
@@ -14799,7 +14799,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B42" s="152" t="s">
+      <c r="B42" s="156" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
@@ -14822,7 +14822,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B43" s="152"/>
+      <c r="B43" s="156"/>
       <c r="C43" t="s">
         <v>150</v>
       </c>
@@ -14843,7 +14843,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B44" s="152"/>
+      <c r="B44" s="156"/>
       <c r="C44" t="s">
         <v>160</v>
       </c>
@@ -14864,7 +14864,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="156" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
@@ -14887,7 +14887,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B46" s="152"/>
+      <c r="B46" s="156"/>
       <c r="C46" t="s">
         <v>150</v>
       </c>
@@ -14908,7 +14908,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B47" s="152"/>
+      <c r="B47" s="156"/>
       <c r="C47" t="s">
         <v>160</v>
       </c>
@@ -14929,7 +14929,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B48" s="152" t="s">
+      <c r="B48" s="156" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
@@ -14952,7 +14952,7 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B49" s="152"/>
+      <c r="B49" s="156"/>
       <c r="C49" t="s">
         <v>150</v>
       </c>
@@ -14973,7 +14973,7 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B50" s="152"/>
+      <c r="B50" s="156"/>
       <c r="C50" t="s">
         <v>160</v>
       </c>
@@ -15018,11 +15018,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -15033,6 +15028,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -29397,8 +29397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29676,7 +29676,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="89">
-        <v>-4.2702871978521627E-5</v>
+        <v>0</v>
       </c>
       <c r="E17" s="85">
         <v>2.7589326302391104E-3</v>

</xml_diff>